<commit_message>
Update: Added Query 203
</commit_message>
<xml_diff>
--- a/requirements/Questions for Tech Board_20Sep18.xlsx
+++ b/requirements/Questions for Tech Board_20Sep18.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pws.mindtree.com/projects/NP-087/Docs/Requirements/Logs-Trackers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100002_{49FC55A8-7080-4BE3-AF48-CCC0C32B719C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_QueryLog_TechBoard" sheetId="5" r:id="rId1"/>
@@ -28,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Vivek Srinivasan</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{16A8D9AB-CA8F-4E38-87FC-7A9B8FFCE7B4}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="118">
   <si>
     <t>MOSIP - QUERY LOG_TechBoard</t>
   </si>
@@ -2357,11 +2356,39 @@
 2. Are authentication type permissions and eKYC permissions tagged to AUA license keys in Aadhaar? What is the expectation from MOSIP?</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Demo De-Duplication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+In Demographic De-duplication, we are supposed to check the demographic details of the packets with other successfully processed packets stored in DataStore/DataBase. 
+1. As we are storing Demographic Data in encrypted format in Database; How are we going to perform Demographic Deduplication for the Packets on Encrypted Data?
+2. How is Data Stored in Aadhaar for Demo Dedupe?</t>
+    </r>
+  </si>
+  <si>
+    <t>User Story - MOS-1064
+Query Log Query - MOS-8589</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -2550,7 +2577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2687,6 +2714,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2968,33 +2998,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:J1"/>
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="37" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="24" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" style="24" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="57" style="4" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="2"/>
-    <col min="13" max="13" width="27.7109375" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="20.28515625" style="1"/>
+    <col min="11" max="11" width="17.54296875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" style="2"/>
+    <col min="13" max="13" width="27.7265625" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="20.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -3011,7 +3041,7 @@
       <c r="L1" s="8"/>
       <c r="M1" s="14"/>
     </row>
-    <row r="2" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3052,7 +3082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="146.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>26</v>
       </c>
@@ -3087,7 +3117,7 @@
       </c>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="161.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>51</v>
       </c>
@@ -3122,7 +3152,7 @@
       </c>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="104.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>53</v>
       </c>
@@ -3157,7 +3187,7 @@
       </c>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="173.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="5" customFormat="1" ht="173.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>55</v>
       </c>
@@ -3192,7 +3222,7 @@
       </c>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="185.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="182" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>56</v>
       </c>
@@ -3227,7 +3257,7 @@
       </c>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="186" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="186" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>76</v>
       </c>
@@ -3262,7 +3292,7 @@
       </c>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="140" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>79</v>
       </c>
@@ -3297,7 +3327,7 @@
       </c>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="126" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>80</v>
       </c>
@@ -3332,7 +3362,7 @@
       </c>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="130.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="130.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>81</v>
       </c>
@@ -3367,7 +3397,7 @@
       </c>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="5" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>82</v>
       </c>
@@ -3402,7 +3432,7 @@
       </c>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="5" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>84</v>
       </c>
@@ -3437,7 +3467,7 @@
       </c>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" s="5" customFormat="1" ht="145.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="5" customFormat="1" ht="145.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>86</v>
       </c>
@@ -3472,7 +3502,7 @@
       </c>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="145.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="145.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>88</v>
       </c>
@@ -3507,7 +3537,7 @@
       </c>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="5" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>93</v>
       </c>
@@ -3542,7 +3572,7 @@
       </c>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>94</v>
       </c>
@@ -3577,7 +3607,7 @@
       </c>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" s="5" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>103</v>
       </c>
@@ -3612,7 +3642,7 @@
       </c>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" s="5" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>124</v>
       </c>
@@ -3647,7 +3677,7 @@
       </c>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" s="5" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="5" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A20" s="35">
         <v>135</v>
       </c>
@@ -3682,7 +3712,7 @@
       </c>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" s="5" customFormat="1" ht="172.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="5" customFormat="1" ht="172.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="35">
         <v>137</v>
       </c>
@@ -3717,7 +3747,7 @@
       </c>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" s="5" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="5" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>141</v>
       </c>
@@ -3752,7 +3782,7 @@
       </c>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" s="5" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="5" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>142</v>
       </c>
@@ -3787,7 +3817,7 @@
       </c>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" s="5" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="5" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>143</v>
       </c>
@@ -3822,7 +3852,7 @@
       </c>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" s="5" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="5" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>153</v>
       </c>
@@ -3857,7 +3887,7 @@
       </c>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" s="5" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="5" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <v>156</v>
       </c>
@@ -3892,7 +3922,7 @@
       </c>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <v>170</v>
       </c>
@@ -3927,7 +3957,7 @@
       </c>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" s="5" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>177</v>
       </c>
@@ -3962,7 +3992,7 @@
       </c>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" s="5" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="5" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>178</v>
       </c>
@@ -3997,7 +4027,7 @@
       </c>
       <c r="M29" s="12"/>
     </row>
-    <row r="30" spans="1:13" s="5" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>179</v>
       </c>
@@ -4032,7 +4062,7 @@
       </c>
       <c r="M30" s="12"/>
     </row>
-    <row r="31" spans="1:13" s="5" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <v>180</v>
       </c>
@@ -4067,7 +4097,7 @@
       </c>
       <c r="M31" s="12"/>
     </row>
-    <row r="32" spans="1:13" s="5" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>181</v>
       </c>
@@ -4098,7 +4128,7 @@
       <c r="L32" s="39"/>
       <c r="M32" s="12"/>
     </row>
-    <row r="33" spans="1:13" s="5" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="5" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A33" s="35">
         <v>183</v>
       </c>
@@ -4129,7 +4159,7 @@
       <c r="L33" s="39"/>
       <c r="M33" s="12"/>
     </row>
-    <row r="34" spans="1:13" s="37" customFormat="1" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="37" customFormat="1" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="35">
         <v>190</v>
       </c>
@@ -4158,7 +4188,7 @@
       <c r="L34" s="9"/>
       <c r="M34" s="12"/>
     </row>
-    <row r="35" spans="1:13" s="37" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="37" customFormat="1" ht="182" x14ac:dyDescent="0.35">
       <c r="A35" s="35">
         <v>191</v>
       </c>
@@ -4187,7 +4217,7 @@
       <c r="L35" s="42"/>
       <c r="M35" s="12"/>
     </row>
-    <row r="36" spans="1:13" s="5" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="5" customFormat="1" ht="238" x14ac:dyDescent="0.35">
       <c r="A36" s="35">
         <v>195</v>
       </c>
@@ -4216,7 +4246,7 @@
       <c r="L36" s="39"/>
       <c r="M36" s="12"/>
     </row>
-    <row r="37" spans="1:13" s="5" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="5" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A37" s="35">
         <v>198</v>
       </c>
@@ -4245,7 +4275,7 @@
       <c r="L37" s="9"/>
       <c r="M37" s="12"/>
     </row>
-    <row r="38" spans="1:13" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <v>199</v>
       </c>
@@ -4274,7 +4304,7 @@
       <c r="L38" s="39"/>
       <c r="M38" s="12"/>
     </row>
-    <row r="39" spans="1:13" ht="171" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="154" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <v>200</v>
       </c>
@@ -4309,7 +4339,7 @@
       <c r="L39" s="39"/>
       <c r="M39" s="12"/>
     </row>
-    <row r="40" spans="1:13" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="84" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>201</v>
       </c>
@@ -4338,7 +4368,7 @@
       <c r="L40" s="39"/>
       <c r="M40" s="12"/>
     </row>
-    <row r="41" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
         <v>202</v>
       </c>
@@ -4367,14 +4397,28 @@
       <c r="L41" s="39"/>
       <c r="M41" s="12"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="16"/>
+    <row r="42" spans="1:13" ht="168" x14ac:dyDescent="0.3">
+      <c r="A42" s="9">
+        <v>203</v>
+      </c>
+      <c r="B42" s="10">
+        <v>43399</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>116</v>
+      </c>
       <c r="H42" s="9"/>
       <c r="I42" s="13"/>
       <c r="J42" s="12"/>
@@ -4382,7 +4426,7 @@
       <c r="L42" s="39"/>
       <c r="M42" s="12"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="10"/>
       <c r="C43" s="9"/>
@@ -4397,7 +4441,7 @@
       <c r="L43" s="40"/>
       <c r="M43" s="12"/>
     </row>
-    <row r="44" spans="1:13" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="143.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="10"/>
       <c r="C44" s="25"/>
@@ -4412,7 +4456,7 @@
       <c r="L44" s="39"/>
       <c r="M44" s="12"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
       <c r="C45" s="9"/>
@@ -4427,7 +4471,7 @@
       <c r="L45" s="39"/>
       <c r="M45" s="12"/>
     </row>
-    <row r="46" spans="1:13" ht="166.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="166.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="10"/>
       <c r="C46" s="9"/>
@@ -4442,7 +4486,7 @@
       <c r="L46" s="10"/>
       <c r="M46" s="12"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
       <c r="C47" s="9"/>
@@ -4457,7 +4501,7 @@
       <c r="L47" s="10"/>
       <c r="M47" s="12"/>
     </row>
-    <row r="48" spans="1:13" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
       <c r="C48" s="25"/>
@@ -4472,7 +4516,7 @@
       <c r="L48" s="10"/>
       <c r="M48" s="12"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="10"/>
       <c r="C49" s="9"/>
@@ -4487,7 +4531,7 @@
       <c r="L49" s="10"/>
       <c r="M49" s="12"/>
     </row>
-    <row r="50" spans="1:13" ht="172.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="172.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
       <c r="B50" s="10"/>
       <c r="C50" s="25"/>
@@ -4502,7 +4546,7 @@
       <c r="L50" s="10"/>
       <c r="M50" s="12"/>
     </row>
-    <row r="51" spans="1:13" ht="181.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="181.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="10"/>
       <c r="C51" s="25"/>
@@ -4517,7 +4561,7 @@
       <c r="L51" s="10"/>
       <c r="M51" s="12"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="10"/>
       <c r="C52" s="9"/>
@@ -4532,7 +4576,7 @@
       <c r="L52" s="10"/>
       <c r="M52" s="12"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="10"/>
       <c r="C53" s="9"/>
@@ -4547,7 +4591,7 @@
       <c r="L53" s="10"/>
       <c r="M53" s="12"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="10"/>
       <c r="C54" s="25"/>
@@ -4562,7 +4606,7 @@
       <c r="L54" s="10"/>
       <c r="M54" s="12"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
       <c r="B55" s="10"/>
       <c r="C55" s="9"/>
@@ -4577,7 +4621,7 @@
       <c r="L55" s="10"/>
       <c r="M55" s="12"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="10"/>
       <c r="C56" s="25"/>
@@ -4592,7 +4636,7 @@
       <c r="L56" s="10"/>
       <c r="M56" s="12"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
       <c r="B57" s="10"/>
       <c r="C57" s="9"/>
@@ -4607,7 +4651,7 @@
       <c r="L57" s="10"/>
       <c r="M57" s="12"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
       <c r="B58" s="10"/>
       <c r="C58" s="25"/>
@@ -4622,7 +4666,7 @@
       <c r="L58" s="10"/>
       <c r="M58" s="12"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="9"/>
@@ -4637,7 +4681,7 @@
       <c r="L59" s="10"/>
       <c r="M59" s="12"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="10"/>
       <c r="C60" s="9"/>
@@ -4652,7 +4696,7 @@
       <c r="L60" s="10"/>
       <c r="M60" s="12"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="10"/>
       <c r="C61" s="25"/>
@@ -4667,7 +4711,7 @@
       <c r="L61" s="10"/>
       <c r="M61" s="12"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="10"/>
       <c r="C62" s="9"/>
@@ -4682,7 +4726,7 @@
       <c r="L62" s="10"/>
       <c r="M62" s="12"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
       <c r="B63" s="10"/>
       <c r="C63" s="9"/>
@@ -4697,7 +4741,7 @@
       <c r="L63" s="10"/>
       <c r="M63" s="12"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
       <c r="B64" s="10"/>
       <c r="C64" s="9"/>
@@ -4712,7 +4756,7 @@
       <c r="L64" s="10"/>
       <c r="M64" s="12"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="9"/>
       <c r="B65" s="10"/>
       <c r="C65" s="9"/>
@@ -4727,7 +4771,7 @@
       <c r="L65" s="10"/>
       <c r="M65" s="12"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="10"/>
       <c r="C66" s="9"/>
@@ -4742,7 +4786,7 @@
       <c r="L66" s="10"/>
       <c r="M66" s="12"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
       <c r="B67" s="10"/>
       <c r="C67" s="9"/>
@@ -4757,7 +4801,7 @@
       <c r="L67" s="10"/>
       <c r="M67" s="12"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="9"/>
       <c r="B68" s="10"/>
       <c r="C68" s="9"/>
@@ -4772,7 +4816,7 @@
       <c r="L68" s="10"/>
       <c r="M68" s="12"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
       <c r="B69" s="10"/>
       <c r="C69" s="9"/>
@@ -4787,7 +4831,7 @@
       <c r="L69" s="10"/>
       <c r="M69" s="12"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="10"/>
       <c r="C70" s="9"/>
@@ -4802,7 +4846,7 @@
       <c r="L70" s="10"/>
       <c r="M70" s="12"/>
     </row>
-    <row r="71" spans="1:13" ht="189.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="189.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="10"/>
       <c r="C71" s="9"/>
@@ -4817,7 +4861,7 @@
       <c r="L71" s="10"/>
       <c r="M71" s="12"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
       <c r="B72" s="10"/>
       <c r="C72" s="9"/>
@@ -4832,7 +4876,7 @@
       <c r="L72" s="10"/>
       <c r="M72" s="12"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="10"/>
       <c r="C73" s="9"/>
@@ -4847,7 +4891,7 @@
       <c r="L73" s="10"/>
       <c r="M73" s="12"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
       <c r="B74" s="10"/>
       <c r="C74" s="9"/>
@@ -4862,7 +4906,7 @@
       <c r="L74" s="10"/>
       <c r="M74" s="12"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>
       <c r="B75" s="10"/>
       <c r="C75" s="9"/>
@@ -4877,7 +4921,7 @@
       <c r="L75" s="10"/>
       <c r="M75" s="12"/>
     </row>
-    <row r="76" spans="1:13" ht="133.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="133.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
       <c r="B76" s="10"/>
       <c r="C76" s="9"/>
@@ -4892,7 +4936,7 @@
       <c r="L76" s="10"/>
       <c r="M76" s="12"/>
     </row>
-    <row r="77" spans="1:13" ht="190.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" ht="190.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="9"/>
       <c r="B77" s="10"/>
       <c r="C77" s="9"/>
@@ -4907,7 +4951,7 @@
       <c r="L77" s="10"/>
       <c r="M77" s="12"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="9"/>
       <c r="B78" s="10"/>
       <c r="C78" s="9"/>
@@ -4922,7 +4966,7 @@
       <c r="L78" s="10"/>
       <c r="M78" s="12"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="9"/>
       <c r="B79" s="10"/>
       <c r="C79" s="9"/>
@@ -4937,7 +4981,7 @@
       <c r="L79" s="10"/>
       <c r="M79" s="12"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="9"/>
       <c r="B80" s="10"/>
       <c r="C80" s="9"/>
@@ -4952,7 +4996,7 @@
       <c r="L80" s="10"/>
       <c r="M80" s="12"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="9"/>
       <c r="B81" s="10"/>
       <c r="C81" s="9"/>
@@ -4967,7 +5011,7 @@
       <c r="L81" s="10"/>
       <c r="M81" s="12"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="9"/>
       <c r="B82" s="10"/>
       <c r="C82" s="9"/>
@@ -4982,7 +5026,7 @@
       <c r="L82" s="10"/>
       <c r="M82" s="12"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="9"/>
       <c r="B83" s="10"/>
       <c r="C83" s="9"/>
@@ -4997,7 +5041,7 @@
       <c r="L83" s="10"/>
       <c r="M83" s="12"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="9"/>
       <c r="B84" s="10"/>
       <c r="C84" s="9"/>
@@ -5012,7 +5056,7 @@
       <c r="L84" s="10"/>
       <c r="M84" s="12"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="B85" s="10"/>
       <c r="C85" s="9"/>
@@ -5027,7 +5071,7 @@
       <c r="L85" s="10"/>
       <c r="M85" s="12"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
       <c r="B86" s="10"/>
       <c r="C86" s="9"/>
@@ -5042,7 +5086,7 @@
       <c r="L86" s="10"/>
       <c r="M86" s="12"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="9"/>
       <c r="B87" s="10"/>
       <c r="C87" s="9"/>
@@ -5057,7 +5101,7 @@
       <c r="L87" s="10"/>
       <c r="M87" s="12"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="9"/>
       <c r="B88" s="10"/>
       <c r="C88" s="9"/>
@@ -5072,7 +5116,7 @@
       <c r="L88" s="10"/>
       <c r="M88" s="12"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="9"/>
       <c r="B89" s="10"/>
       <c r="C89" s="9"/>
@@ -5087,7 +5131,7 @@
       <c r="L89" s="10"/>
       <c r="M89" s="12"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="9"/>
       <c r="B90" s="10"/>
       <c r="C90" s="9"/>
@@ -5102,7 +5146,7 @@
       <c r="L90" s="10"/>
       <c r="M90" s="12"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="9"/>
       <c r="B91" s="10"/>
       <c r="C91" s="9"/>
@@ -5117,7 +5161,7 @@
       <c r="L91" s="10"/>
       <c r="M91" s="12"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="9"/>
       <c r="B92" s="10"/>
       <c r="C92" s="9"/>
@@ -5132,7 +5176,7 @@
       <c r="L92" s="10"/>
       <c r="M92" s="12"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
       <c r="B93" s="10"/>
       <c r="C93" s="9"/>
@@ -5147,7 +5191,7 @@
       <c r="L93" s="10"/>
       <c r="M93" s="12"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="10"/>
       <c r="C94" s="9"/>
@@ -5162,7 +5206,7 @@
       <c r="L94" s="10"/>
       <c r="M94" s="12"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
       <c r="B95" s="10"/>
       <c r="C95" s="9"/>
@@ -5177,7 +5221,7 @@
       <c r="L95" s="10"/>
       <c r="M95" s="12"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="9"/>
       <c r="B96" s="10"/>
       <c r="C96" s="9"/>
@@ -5192,7 +5236,7 @@
       <c r="L96" s="10"/>
       <c r="M96" s="12"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="9"/>
       <c r="B97" s="10"/>
       <c r="C97" s="9"/>
@@ -5207,7 +5251,7 @@
       <c r="L97" s="10"/>
       <c r="M97" s="12"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="9"/>
       <c r="B98" s="10"/>
       <c r="C98" s="9"/>
@@ -5222,7 +5266,7 @@
       <c r="L98" s="9"/>
       <c r="M98" s="12"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="9"/>
       <c r="B99" s="10"/>
       <c r="C99" s="9"/>
@@ -5237,7 +5281,7 @@
       <c r="L99" s="10"/>
       <c r="M99" s="12"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="9"/>
       <c r="B100" s="10"/>
       <c r="C100" s="9"/>
@@ -5252,7 +5296,7 @@
       <c r="L100" s="10"/>
       <c r="M100" s="12"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="9"/>
       <c r="B101" s="10"/>
       <c r="C101" s="9"/>
@@ -5267,7 +5311,7 @@
       <c r="L101" s="10"/>
       <c r="M101" s="12"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="9"/>
       <c r="B102" s="10"/>
       <c r="C102" s="9"/>
@@ -5282,7 +5326,7 @@
       <c r="L102" s="10"/>
       <c r="M102" s="12"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="9"/>
       <c r="B103" s="10"/>
       <c r="C103" s="9"/>
@@ -5297,7 +5341,7 @@
       <c r="L103" s="10"/>
       <c r="M103" s="12"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="9"/>
       <c r="B104" s="10"/>
       <c r="C104" s="9"/>
@@ -5312,7 +5356,7 @@
       <c r="L104" s="10"/>
       <c r="M104" s="12"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="9"/>
       <c r="B105" s="10"/>
       <c r="C105" s="9"/>
@@ -5327,7 +5371,7 @@
       <c r="L105" s="10"/>
       <c r="M105" s="12"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="9"/>
       <c r="B106" s="10"/>
       <c r="C106" s="9"/>
@@ -5342,7 +5386,7 @@
       <c r="L106" s="10"/>
       <c r="M106" s="12"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="9"/>
       <c r="B107" s="10"/>
       <c r="C107" s="9"/>
@@ -5357,7 +5401,7 @@
       <c r="L107" s="10"/>
       <c r="M107" s="12"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="9"/>
       <c r="B108" s="10"/>
       <c r="C108" s="9"/>
@@ -5372,7 +5416,7 @@
       <c r="L108" s="10"/>
       <c r="M108" s="12"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="9"/>
       <c r="B109" s="10"/>
       <c r="C109" s="9"/>
@@ -5387,7 +5431,7 @@
       <c r="L109" s="10"/>
       <c r="M109" s="12"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="9"/>
       <c r="B110" s="10"/>
       <c r="C110" s="9"/>
@@ -5402,7 +5446,7 @@
       <c r="L110" s="10"/>
       <c r="M110" s="12"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="9"/>
       <c r="B111" s="10"/>
       <c r="C111" s="9"/>
@@ -5417,7 +5461,7 @@
       <c r="L111" s="10"/>
       <c r="M111" s="12"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="9"/>
       <c r="B112" s="10"/>
       <c r="C112" s="9"/>
@@ -5432,7 +5476,7 @@
       <c r="L112" s="10"/>
       <c r="M112" s="12"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="9"/>
       <c r="B113" s="10"/>
       <c r="C113" s="9"/>
@@ -5447,7 +5491,7 @@
       <c r="L113" s="10"/>
       <c r="M113" s="12"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="9"/>
       <c r="B114" s="10"/>
       <c r="C114" s="9"/>
@@ -5462,7 +5506,7 @@
       <c r="L114" s="10"/>
       <c r="M114" s="12"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="9"/>
       <c r="B115" s="10"/>
       <c r="C115" s="9"/>
@@ -5477,7 +5521,7 @@
       <c r="L115" s="10"/>
       <c r="M115" s="12"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="9"/>
       <c r="B116" s="10"/>
       <c r="C116" s="9"/>
@@ -5492,7 +5536,7 @@
       <c r="L116" s="10"/>
       <c r="M116" s="12"/>
     </row>
-    <row r="117" spans="1:13" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="9"/>
       <c r="B117" s="10"/>
       <c r="C117" s="9"/>
@@ -5507,7 +5551,7 @@
       <c r="L117" s="10"/>
       <c r="M117" s="12"/>
     </row>
-    <row r="118" spans="1:13" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="9"/>
       <c r="B118" s="10"/>
       <c r="C118" s="9"/>
@@ -5522,7 +5566,7 @@
       <c r="L118" s="10"/>
       <c r="M118" s="12"/>
     </row>
-    <row r="119" spans="1:13" ht="103.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" ht="103.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="9"/>
       <c r="B119" s="10"/>
       <c r="C119" s="9"/>
@@ -5537,7 +5581,7 @@
       <c r="L119" s="10"/>
       <c r="M119" s="12"/>
     </row>
-    <row r="120" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="9"/>
       <c r="B120" s="10"/>
       <c r="C120" s="9"/>
@@ -5552,7 +5596,7 @@
       <c r="L120" s="10"/>
       <c r="M120" s="12"/>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="9"/>
       <c r="B121" s="10"/>
       <c r="C121" s="9"/>
@@ -5567,7 +5611,7 @@
       <c r="L121" s="10"/>
       <c r="M121" s="12"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="9"/>
       <c r="B122" s="10"/>
       <c r="C122" s="9"/>
@@ -5582,7 +5626,7 @@
       <c r="L122" s="10"/>
       <c r="M122" s="12"/>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="9"/>
       <c r="B123" s="10"/>
       <c r="C123" s="9"/>
@@ -5597,7 +5641,7 @@
       <c r="L123" s="9"/>
       <c r="M123" s="12"/>
     </row>
-    <row r="124" spans="1:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="42.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="9"/>
       <c r="B124" s="10"/>
       <c r="C124" s="9"/>
@@ -5612,7 +5656,7 @@
       <c r="L124" s="9"/>
       <c r="M124" s="12"/>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="9"/>
       <c r="B125" s="10"/>
       <c r="C125" s="9"/>
@@ -5627,7 +5671,7 @@
       <c r="L125" s="9"/>
       <c r="M125" s="12"/>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="9"/>
       <c r="B126" s="10"/>
       <c r="C126" s="9"/>
@@ -5642,7 +5686,7 @@
       <c r="L126" s="9"/>
       <c r="M126" s="12"/>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="9"/>
       <c r="B127" s="10"/>
       <c r="C127" s="9"/>
@@ -5657,7 +5701,7 @@
       <c r="L127" s="9"/>
       <c r="M127" s="12"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="9"/>
       <c r="B128" s="10"/>
       <c r="C128" s="9"/>
@@ -5672,7 +5716,7 @@
       <c r="L128" s="9"/>
       <c r="M128" s="12"/>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="9"/>
       <c r="B129" s="10"/>
       <c r="C129" s="9"/>
@@ -5687,7 +5731,7 @@
       <c r="L129" s="9"/>
       <c r="M129" s="12"/>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="35"/>
       <c r="B130" s="10"/>
       <c r="C130" s="9"/>
@@ -5702,7 +5746,7 @@
       <c r="L130" s="9"/>
       <c r="M130" s="12"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="35"/>
       <c r="B131" s="10"/>
       <c r="C131" s="9"/>
@@ -5717,7 +5761,7 @@
       <c r="L131" s="9"/>
       <c r="M131" s="12"/>
     </row>
-    <row r="132" spans="1:13" ht="170.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" ht="170.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="35"/>
       <c r="B132" s="10"/>
       <c r="C132" s="9"/>
@@ -5732,7 +5776,7 @@
       <c r="L132" s="9"/>
       <c r="M132" s="12"/>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="35"/>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
@@ -5747,7 +5791,7 @@
       <c r="L133" s="9"/>
       <c r="M133" s="12"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="35"/>
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
@@ -5762,7 +5806,7 @@
       <c r="L134" s="9"/>
       <c r="M134" s="12"/>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" s="35"/>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -5777,7 +5821,7 @@
       <c r="L135" s="9"/>
       <c r="M135" s="12"/>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" s="35"/>
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
@@ -5793,7 +5837,7 @@
       <c r="M136" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:M32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:M32"/>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
@@ -5804,41 +5848,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6045,32 +6054,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1DD169-1613-4852-8D49-4C3CB1FDBF80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6087,4 +6106,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>